<commit_message>
boast xlsx nit update
</commit_message>
<xml_diff>
--- a/content/boasts.xlsx
+++ b/content/boasts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgu/pear/backend-graphql/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45F6B67-EE04-FE4C-A03E-6D9D3FEB94A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F546D7-F641-CD44-B464-01919903D15F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{8DA4199E-1993-0447-8C09-83FBCB57DFF9}"/>
   </bookViews>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F06EFA9-AFB9-2748-A0FB-6DB13774CB33}">
   <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2332,10 +2332,10 @@
         <v>129</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>